<commit_message>
Initial working notional build.
</commit_message>
<xml_diff>
--- a/test/resources/usage/timeline_A.xlsx
+++ b/test/resources/usage/timeline_A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://armyeitaas-my.sharepoint-mil.us/personal/thomas_l_spoon_civ_army_mil/Documents/Documents/notional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8FD941E-ED3D-4189-8FF5-6598D46185A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{E8FD941E-ED3D-4189-8FF5-6598D46185A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD322BAB-2BEF-46D3-BAE7-B23286D91C4D}"/>
   <bookViews>
-    <workbookView xWindow="29715" yWindow="1005" windowWidth="27165" windowHeight="14205" xr2:uid="{1EAEDFC6-FFEF-4692-871C-22CBD34688C2}"/>
+    <workbookView xWindow="4785" yWindow="2040" windowWidth="23010" windowHeight="12195" xr2:uid="{1EAEDFC6-FFEF-4692-871C-22CBD34688C2}"/>
   </bookViews>
   <sheets>
     <sheet name="New-map-format" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>ForceCode</t>
   </si>
   <si>
-    <t>Alpha</t>
-  </si>
-  <si>
     <t>Rotational</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>SE-A</t>
   </si>
 </sst>
 </file>
@@ -121,6 +121,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,32 +447,32 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>1335</v>
@@ -477,9 +481,9 @@
         <v>981</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -488,9 +492,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -499,9 +503,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>2316</v>
@@ -510,9 +514,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>2316</v>
@@ -521,9 +525,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>1335</v>
@@ -532,9 +536,9 @@
         <v>981</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -543,9 +547,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -554,9 +558,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>2316</v>
@@ -565,9 +569,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>2316</v>
@@ -576,9 +580,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -587,9 +591,9 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>2316</v>
@@ -601,4 +605,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{554eecc5-e26c-4620-b240-5a8bb326c33d}" enabled="1" method="Privileged" siteId="{fae6d70f-954b-4811-92b6-0530d6f84c43}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>